<commit_message>
update Rmd to v5
added carryover/TDM section, reduced expansion to a single (mean) value, focused on Aug-Sept volume instead of Aug-Oct.
</commit_message>
<xml_diff>
--- a/External_data/FlowScen/FallFlows20240826_V2_Draft.xlsx
+++ b/External_data/FlowScen/FallFlows20240826_V2_Draft.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cehlo_usbr_gov/Documents/Redd_dewatering/Fall_Flow_Redd_Dewatering/External_data/FlowScen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/lelliott_usbr_gov/Documents/Documents/GitHub/BDO-Science/Fall_Flow_Redd_Dewatering/External_data/FlowScen/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="67" documentId="8_{716FE34C-2D26-4FFD-A9D5-19040DD9C17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C01E4AA8-D3A5-4783-ADE8-639FC460E04D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="876" activeTab="5" xr2:uid="{8B6B0201-DD1B-4D0A-8FA2-1793C828B1EC}"/>
+    <workbookView xWindow="-25515" yWindow="2325" windowWidth="21600" windowHeight="11385" tabRatio="876" activeTab="5" xr2:uid="{8B6B0201-DD1B-4D0A-8FA2-1793C828B1EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Keswick Flow Alternatives" sheetId="3" r:id="rId1"/>
@@ -1774,38 +1774,6 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1833,6 +1801,38 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="126">
     <cellStyle name="Comma 10" xfId="86" xr:uid="{18F22F41-CF6B-4170-A614-400F6543E9A0}"/>
@@ -8885,28 +8885,28 @@
                   <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>10000000</c:v>
@@ -13932,28 +13932,28 @@
                   <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>10000000</c:v>
@@ -18527,7 +18527,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B9A0DFFB-0EAB-4130-A4A2-055D67D97DCF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="68" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18538,7 +18538,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{14D33800-CE90-42EF-8DBE-41B375C6FC84}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="68" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18615,7 +18615,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8664087" cy="6288942"/>
+    <xdr:ext cx="8682935" cy="6308587"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -18648,7 +18648,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663983" cy="6290805"/>
+    <xdr:ext cx="8682935" cy="6308587"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -18675,10 +18675,6 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18981,31 +18977,31 @@
   <dimension ref="A1:O242"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E227" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="22" customWidth="1"/>
-    <col min="3" max="5" width="14.5546875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="14.5546875" style="22" customWidth="1"/>
-    <col min="15" max="15" width="8.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.5546875" style="22"/>
+    <col min="1" max="1" width="28.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="22" customWidth="1"/>
+    <col min="3" max="5" width="14.5703125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="14.5703125" style="22" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.5703125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="30"/>
     </row>
-    <row r="2" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -19039,7 +19035,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="43">
         <f t="shared" ref="A3:A32" si="0">A4-1</f>
         <v>45505</v>
@@ -19076,7 +19072,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="43">
         <f t="shared" si="0"/>
         <v>45506</v>
@@ -19119,7 +19115,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43">
         <f t="shared" si="0"/>
         <v>45507</v>
@@ -19162,7 +19158,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="43">
         <f t="shared" si="0"/>
         <v>45508</v>
@@ -19205,7 +19201,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="43">
         <f t="shared" si="0"/>
         <v>45509</v>
@@ -19248,7 +19244,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="43">
         <f t="shared" si="0"/>
         <v>45510</v>
@@ -19291,7 +19287,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="43">
         <f t="shared" si="0"/>
         <v>45511</v>
@@ -19334,7 +19330,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="43">
         <f t="shared" si="0"/>
         <v>45512</v>
@@ -19377,7 +19373,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="43">
         <f t="shared" si="0"/>
         <v>45513</v>
@@ -19420,7 +19416,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="43">
         <f t="shared" si="0"/>
         <v>45514</v>
@@ -19463,7 +19459,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="43">
         <f t="shared" si="0"/>
         <v>45515</v>
@@ -19506,7 +19502,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="43">
         <f t="shared" si="0"/>
         <v>45516</v>
@@ -19549,7 +19545,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="43">
         <f t="shared" si="0"/>
         <v>45517</v>
@@ -19592,7 +19588,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="43">
         <f t="shared" si="0"/>
         <v>45518</v>
@@ -19635,7 +19631,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43">
         <f t="shared" si="0"/>
         <v>45519</v>
@@ -19678,7 +19674,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43">
         <f t="shared" si="0"/>
         <v>45520</v>
@@ -19721,7 +19717,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43">
         <f t="shared" si="0"/>
         <v>45521</v>
@@ -19764,7 +19760,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43">
         <f t="shared" si="0"/>
         <v>45522</v>
@@ -19807,7 +19803,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="43">
         <f t="shared" si="0"/>
         <v>45523</v>
@@ -19850,7 +19846,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="43">
         <f t="shared" si="0"/>
         <v>45524</v>
@@ -19893,7 +19889,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="43">
         <f t="shared" si="0"/>
         <v>45525</v>
@@ -19936,7 +19932,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="43">
         <f t="shared" si="0"/>
         <v>45526</v>
@@ -19979,7 +19975,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="43">
         <f t="shared" si="0"/>
         <v>45527</v>
@@ -20022,7 +20018,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="43">
         <f t="shared" si="0"/>
         <v>45528</v>
@@ -20065,7 +20061,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="43">
         <f t="shared" si="0"/>
         <v>45529</v>
@@ -20108,7 +20104,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="43">
         <f t="shared" si="0"/>
         <v>45530</v>
@@ -20151,7 +20147,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="43">
         <f t="shared" si="0"/>
         <v>45531</v>
@@ -20191,10 +20187,10 @@
       <c r="N29" s="22"/>
       <c r="O29" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="43">
         <f t="shared" si="0"/>
         <v>45532</v>
@@ -20234,10 +20230,10 @@
       <c r="N30" s="22"/>
       <c r="O30" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="43">
         <f t="shared" si="0"/>
         <v>45533</v>
@@ -20277,10 +20273,10 @@
       <c r="N31" s="22"/>
       <c r="O31" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="43">
         <f t="shared" si="0"/>
         <v>45534</v>
@@ -20320,10 +20316,10 @@
       <c r="N32" s="22"/>
       <c r="O32" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="44">
         <f>A34-1</f>
         <v>45535</v>
@@ -20363,10 +20359,10 @@
       <c r="N33" s="22"/>
       <c r="O33" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="57">
         <v>45536</v>
       </c>
@@ -20397,10 +20393,10 @@
       <c r="N34" s="22"/>
       <c r="O34" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="45">
         <f>A34+1</f>
         <v>45537</v>
@@ -20438,10 +20434,10 @@
       <c r="N35" s="22"/>
       <c r="O35" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="45">
         <f t="shared" ref="A36:A99" si="63">A35+1</f>
         <v>45538</v>
@@ -20479,10 +20475,10 @@
       <c r="N36" s="22"/>
       <c r="O36" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="45">
         <f t="shared" si="63"/>
         <v>45539</v>
@@ -20523,7 +20519,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="45">
         <f t="shared" si="63"/>
         <v>45540</v>
@@ -20564,7 +20560,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="45">
         <f t="shared" si="63"/>
         <v>45541</v>
@@ -20605,7 +20601,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="45">
         <f t="shared" si="63"/>
         <v>45542</v>
@@ -20646,7 +20642,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="45">
         <f t="shared" si="63"/>
         <v>45543</v>
@@ -20687,7 +20683,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="45">
         <f t="shared" si="63"/>
         <v>45544</v>
@@ -20728,7 +20724,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="45">
         <f t="shared" si="63"/>
         <v>45545</v>
@@ -20769,7 +20765,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="45">
         <f t="shared" si="63"/>
         <v>45546</v>
@@ -20810,7 +20806,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="45">
         <f t="shared" si="63"/>
         <v>45547</v>
@@ -20851,7 +20847,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="45">
         <f t="shared" si="63"/>
         <v>45548</v>
@@ -20892,7 +20888,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="45">
         <f t="shared" si="63"/>
         <v>45549</v>
@@ -20933,7 +20929,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="45">
         <f t="shared" si="63"/>
         <v>45550</v>
@@ -20974,7 +20970,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="45">
         <f t="shared" si="63"/>
         <v>45551</v>
@@ -21015,7 +21011,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="45">
         <f t="shared" si="63"/>
         <v>45552</v>
@@ -21056,7 +21052,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="45">
         <f t="shared" si="63"/>
         <v>45553</v>
@@ -21097,7 +21093,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="45">
         <f t="shared" si="63"/>
         <v>45554</v>
@@ -21138,7 +21134,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="45">
         <f t="shared" si="63"/>
         <v>45555</v>
@@ -21179,7 +21175,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="45">
         <f t="shared" si="63"/>
         <v>45556</v>
@@ -21220,7 +21216,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="45">
         <f t="shared" si="63"/>
         <v>45557</v>
@@ -21261,7 +21257,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="45">
         <f t="shared" si="63"/>
         <v>45558</v>
@@ -21302,7 +21298,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="45">
         <f t="shared" si="63"/>
         <v>45559</v>
@@ -21343,7 +21339,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="45">
         <f t="shared" si="63"/>
         <v>45560</v>
@@ -21384,7 +21380,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="45">
         <f t="shared" si="63"/>
         <v>45561</v>
@@ -21425,7 +21421,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="45">
         <f t="shared" si="63"/>
         <v>45562</v>
@@ -21466,7 +21462,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="45">
         <f t="shared" si="63"/>
         <v>45563</v>
@@ -21507,7 +21503,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="45">
         <f t="shared" si="63"/>
         <v>45564</v>
@@ -21548,7 +21544,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="45">
         <f t="shared" si="63"/>
         <v>45565</v>
@@ -21589,7 +21585,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="65">
         <f t="shared" si="63"/>
         <v>45566</v>
@@ -21624,7 +21620,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="45">
         <f t="shared" si="63"/>
         <v>45567</v>
@@ -21665,7 +21661,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="45">
         <f t="shared" si="63"/>
         <v>45568</v>
@@ -21706,7 +21702,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="45">
         <f t="shared" si="63"/>
         <v>45569</v>
@@ -21747,7 +21743,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="45">
         <f t="shared" si="63"/>
         <v>45570</v>
@@ -21788,7 +21784,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="45">
         <f t="shared" si="63"/>
         <v>45571</v>
@@ -21829,7 +21825,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="45">
         <f t="shared" si="63"/>
         <v>45572</v>
@@ -21870,7 +21866,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="45">
         <f t="shared" si="63"/>
         <v>45573</v>
@@ -21911,7 +21907,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="45">
         <f t="shared" si="63"/>
         <v>45574</v>
@@ -21952,7 +21948,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="45">
         <f t="shared" si="63"/>
         <v>45575</v>
@@ -21993,7 +21989,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="45">
         <f t="shared" si="63"/>
         <v>45576</v>
@@ -22034,7 +22030,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="45">
         <f t="shared" si="63"/>
         <v>45577</v>
@@ -22075,7 +22071,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="45">
         <f t="shared" si="63"/>
         <v>45578</v>
@@ -22116,7 +22112,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="45">
         <f t="shared" si="63"/>
         <v>45579</v>
@@ -22157,7 +22153,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="45">
         <f t="shared" si="63"/>
         <v>45580</v>
@@ -22198,7 +22194,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="45">
         <f t="shared" si="63"/>
         <v>45581</v>
@@ -22239,7 +22235,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="45">
         <f t="shared" si="63"/>
         <v>45582</v>
@@ -22280,7 +22276,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="45">
         <f t="shared" si="63"/>
         <v>45583</v>
@@ -22321,7 +22317,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="45">
         <f t="shared" si="63"/>
         <v>45584</v>
@@ -22362,7 +22358,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="45">
         <f t="shared" si="63"/>
         <v>45585</v>
@@ -22403,7 +22399,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="45">
         <f t="shared" si="63"/>
         <v>45586</v>
@@ -22444,7 +22440,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="45">
         <f t="shared" si="63"/>
         <v>45587</v>
@@ -22485,7 +22481,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="45">
         <f t="shared" si="63"/>
         <v>45588</v>
@@ -22526,7 +22522,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="45">
         <f t="shared" si="63"/>
         <v>45589</v>
@@ -22567,7 +22563,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="45">
         <f t="shared" si="63"/>
         <v>45590</v>
@@ -22608,7 +22604,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="45">
         <f t="shared" si="63"/>
         <v>45591</v>
@@ -22649,7 +22645,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="45">
         <f t="shared" si="63"/>
         <v>45592</v>
@@ -22690,7 +22686,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="45">
         <f t="shared" si="63"/>
         <v>45593</v>
@@ -22731,7 +22727,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="45">
         <f t="shared" si="63"/>
         <v>45594</v>
@@ -22772,7 +22768,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="45">
         <f t="shared" si="63"/>
         <v>45595</v>
@@ -22813,7 +22809,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="45">
         <f t="shared" si="63"/>
         <v>45596</v>
@@ -22854,7 +22850,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="65">
         <f t="shared" si="63"/>
         <v>45597</v>
@@ -22889,7 +22885,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="46">
         <f t="shared" si="63"/>
         <v>45598</v>
@@ -22929,7 +22925,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="46">
         <f t="shared" si="63"/>
         <v>45599</v>
@@ -22969,7 +22965,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="46">
         <f t="shared" si="63"/>
         <v>45600</v>
@@ -23009,7 +23005,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="46">
         <f t="shared" si="63"/>
         <v>45601</v>
@@ -23049,7 +23045,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="46">
         <f t="shared" ref="A100:A163" si="194">A99+1</f>
         <v>45602</v>
@@ -23089,7 +23085,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="46">
         <f t="shared" si="194"/>
         <v>45603</v>
@@ -23129,7 +23125,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="46">
         <f t="shared" si="194"/>
         <v>45604</v>
@@ -23169,7 +23165,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="46">
         <f t="shared" si="194"/>
         <v>45605</v>
@@ -23209,7 +23205,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="46">
         <f t="shared" si="194"/>
         <v>45606</v>
@@ -23249,7 +23245,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="46">
         <f t="shared" si="194"/>
         <v>45607</v>
@@ -23289,7 +23285,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="46">
         <f t="shared" si="194"/>
         <v>45608</v>
@@ -23329,7 +23325,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="46">
         <f t="shared" si="194"/>
         <v>45609</v>
@@ -23368,7 +23364,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="46">
         <f t="shared" si="194"/>
         <v>45610</v>
@@ -23409,7 +23405,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="46">
         <f t="shared" si="194"/>
         <v>45611</v>
@@ -23450,7 +23446,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="46">
         <f t="shared" si="194"/>
         <v>45612</v>
@@ -23491,7 +23487,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="46">
         <f t="shared" si="194"/>
         <v>45613</v>
@@ -23532,7 +23528,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="46">
         <f t="shared" si="194"/>
         <v>45614</v>
@@ -23573,7 +23569,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="46">
         <f t="shared" si="194"/>
         <v>45615</v>
@@ -23614,7 +23610,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="46">
         <f t="shared" si="194"/>
         <v>45616</v>
@@ -23655,7 +23651,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="46">
         <f t="shared" si="194"/>
         <v>45617</v>
@@ -23696,7 +23692,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="46">
         <f t="shared" si="194"/>
         <v>45618</v>
@@ -23737,7 +23733,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="46">
         <f t="shared" si="194"/>
         <v>45619</v>
@@ -23778,7 +23774,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="46">
         <f t="shared" si="194"/>
         <v>45620</v>
@@ -23819,7 +23815,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="46">
         <f t="shared" si="194"/>
         <v>45621</v>
@@ -23860,7 +23856,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="46">
         <f t="shared" si="194"/>
         <v>45622</v>
@@ -23901,7 +23897,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="46">
         <f t="shared" si="194"/>
         <v>45623</v>
@@ -23942,7 +23938,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="46">
         <f t="shared" si="194"/>
         <v>45624</v>
@@ -23983,7 +23979,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="46">
         <f t="shared" si="194"/>
         <v>45625</v>
@@ -24024,7 +24020,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="47">
         <f t="shared" si="194"/>
         <v>45626</v>
@@ -24065,7 +24061,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="57">
         <f t="shared" si="194"/>
         <v>45627</v>
@@ -24100,7 +24096,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="45">
         <f t="shared" si="194"/>
         <v>45628</v>
@@ -24141,7 +24137,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="45">
         <f t="shared" si="194"/>
         <v>45629</v>
@@ -24182,7 +24178,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="45">
         <f t="shared" si="194"/>
         <v>45630</v>
@@ -24223,7 +24219,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="45">
         <f t="shared" si="194"/>
         <v>45631</v>
@@ -24264,7 +24260,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="45">
         <f t="shared" si="194"/>
         <v>45632</v>
@@ -24305,7 +24301,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="45">
         <f t="shared" si="194"/>
         <v>45633</v>
@@ -24346,7 +24342,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" s="45">
         <f t="shared" si="194"/>
         <v>45634</v>
@@ -24387,7 +24383,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" s="45">
         <f t="shared" si="194"/>
         <v>45635</v>
@@ -24428,7 +24424,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="45">
         <f t="shared" si="194"/>
         <v>45636</v>
@@ -24469,7 +24465,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="45">
         <f t="shared" si="194"/>
         <v>45637</v>
@@ -24510,7 +24506,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="45">
         <f t="shared" si="194"/>
         <v>45638</v>
@@ -24551,7 +24547,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" s="45">
         <f t="shared" si="194"/>
         <v>45639</v>
@@ -24592,7 +24588,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" s="45">
         <f t="shared" si="194"/>
         <v>45640</v>
@@ -24633,7 +24629,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" s="45">
         <f t="shared" si="194"/>
         <v>45641</v>
@@ -24674,7 +24670,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" s="45">
         <f t="shared" si="194"/>
         <v>45642</v>
@@ -24715,7 +24711,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" s="45">
         <f t="shared" si="194"/>
         <v>45643</v>
@@ -24756,7 +24752,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="45">
         <f t="shared" si="194"/>
         <v>45644</v>
@@ -24797,7 +24793,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="45">
         <f t="shared" si="194"/>
         <v>45645</v>
@@ -24838,7 +24834,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" s="45">
         <f t="shared" si="194"/>
         <v>45646</v>
@@ -24879,7 +24875,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" s="45">
         <f t="shared" si="194"/>
         <v>45647</v>
@@ -24920,7 +24916,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" s="45">
         <f t="shared" si="194"/>
         <v>45648</v>
@@ -24961,7 +24957,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" s="45">
         <f t="shared" si="194"/>
         <v>45649</v>
@@ -25002,7 +24998,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" s="45">
         <f t="shared" si="194"/>
         <v>45650</v>
@@ -25043,7 +25039,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" s="45">
         <f t="shared" si="194"/>
         <v>45651</v>
@@ -25084,7 +25080,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" s="45">
         <f t="shared" si="194"/>
         <v>45652</v>
@@ -25125,7 +25121,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" s="45">
         <f t="shared" si="194"/>
         <v>45653</v>
@@ -25166,7 +25162,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" s="45">
         <f t="shared" si="194"/>
         <v>45654</v>
@@ -25207,7 +25203,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" s="45">
         <f t="shared" si="194"/>
         <v>45655</v>
@@ -25248,7 +25244,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" s="45">
         <f t="shared" si="194"/>
         <v>45656</v>
@@ -25289,7 +25285,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" s="45">
         <f t="shared" si="194"/>
         <v>45657</v>
@@ -25330,7 +25326,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" s="65">
         <f t="shared" si="194"/>
         <v>45658</v>
@@ -25365,7 +25361,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" s="46">
         <f t="shared" si="194"/>
         <v>45659</v>
@@ -25406,7 +25402,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" s="46">
         <f t="shared" si="194"/>
         <v>45660</v>
@@ -25447,7 +25443,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" s="46">
         <f t="shared" si="194"/>
         <v>45661</v>
@@ -25488,7 +25484,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" s="46">
         <f t="shared" si="194"/>
         <v>45662</v>
@@ -25529,7 +25525,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" s="46">
         <f t="shared" si="194"/>
         <v>45663</v>
@@ -25570,7 +25566,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" s="46">
         <f t="shared" si="194"/>
         <v>45664</v>
@@ -25611,7 +25607,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" s="46">
         <f t="shared" si="194"/>
         <v>45665</v>
@@ -25652,7 +25648,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" s="46">
         <f t="shared" ref="A164:A214" si="384">A163+1</f>
         <v>45666</v>
@@ -25693,7 +25689,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" s="46">
         <f t="shared" si="384"/>
         <v>45667</v>
@@ -25734,7 +25730,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" s="46">
         <f t="shared" si="384"/>
         <v>45668</v>
@@ -25775,7 +25771,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" s="46">
         <f t="shared" si="384"/>
         <v>45669</v>
@@ -25816,7 +25812,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" s="46">
         <f t="shared" si="384"/>
         <v>45670</v>
@@ -25857,7 +25853,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" s="46">
         <f t="shared" si="384"/>
         <v>45671</v>
@@ -25898,7 +25894,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" s="46">
         <f t="shared" si="384"/>
         <v>45672</v>
@@ -25939,7 +25935,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A171" s="46">
         <f t="shared" si="384"/>
         <v>45673</v>
@@ -25980,7 +25976,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" s="46">
         <f t="shared" si="384"/>
         <v>45674</v>
@@ -26021,7 +26017,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" s="46">
         <f t="shared" si="384"/>
         <v>45675</v>
@@ -26062,7 +26058,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" s="46">
         <f t="shared" si="384"/>
         <v>45676</v>
@@ -26103,7 +26099,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A175" s="46">
         <f t="shared" si="384"/>
         <v>45677</v>
@@ -26144,7 +26140,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A176" s="46">
         <f t="shared" si="384"/>
         <v>45678</v>
@@ -26185,7 +26181,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A177" s="46">
         <f t="shared" si="384"/>
         <v>45679</v>
@@ -26226,7 +26222,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A178" s="46">
         <f t="shared" si="384"/>
         <v>45680</v>
@@ -26267,7 +26263,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A179" s="46">
         <f t="shared" si="384"/>
         <v>45681</v>
@@ -26308,7 +26304,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A180" s="46">
         <f t="shared" si="384"/>
         <v>45682</v>
@@ -26349,7 +26345,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A181" s="46">
         <f t="shared" si="384"/>
         <v>45683</v>
@@ -26390,7 +26386,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A182" s="46">
         <f t="shared" si="384"/>
         <v>45684</v>
@@ -26431,7 +26427,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" s="46">
         <f t="shared" si="384"/>
         <v>45685</v>
@@ -26472,7 +26468,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A184" s="46">
         <f t="shared" si="384"/>
         <v>45686</v>
@@ -26513,7 +26509,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A185" s="46">
         <f t="shared" si="384"/>
         <v>45687</v>
@@ -26554,7 +26550,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A186" s="47">
         <f t="shared" si="384"/>
         <v>45688</v>
@@ -26595,7 +26591,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A187" s="57">
         <f t="shared" si="384"/>
         <v>45689</v>
@@ -26630,7 +26626,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A188" s="45">
         <f t="shared" si="384"/>
         <v>45690</v>
@@ -26671,7 +26667,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" s="45">
         <f t="shared" si="384"/>
         <v>45691</v>
@@ -26712,7 +26708,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A190" s="45">
         <f t="shared" si="384"/>
         <v>45692</v>
@@ -26753,7 +26749,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" s="45">
         <f t="shared" si="384"/>
         <v>45693</v>
@@ -26794,7 +26790,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A192" s="45">
         <f t="shared" si="384"/>
         <v>45694</v>
@@ -26835,7 +26831,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A193" s="45">
         <f t="shared" si="384"/>
         <v>45695</v>
@@ -26876,7 +26872,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A194" s="45">
         <f t="shared" si="384"/>
         <v>45696</v>
@@ -26917,7 +26913,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A195" s="45">
         <f t="shared" si="384"/>
         <v>45697</v>
@@ -26958,7 +26954,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" s="45">
         <f t="shared" si="384"/>
         <v>45698</v>
@@ -26999,7 +26995,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A197" s="45">
         <f t="shared" si="384"/>
         <v>45699</v>
@@ -27040,7 +27036,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A198" s="45">
         <f t="shared" si="384"/>
         <v>45700</v>
@@ -27081,7 +27077,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A199" s="45">
         <f t="shared" si="384"/>
         <v>45701</v>
@@ -27122,7 +27118,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A200" s="45">
         <f t="shared" si="384"/>
         <v>45702</v>
@@ -27163,7 +27159,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A201" s="45">
         <f t="shared" si="384"/>
         <v>45703</v>
@@ -27204,7 +27200,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" s="45">
         <f t="shared" si="384"/>
         <v>45704</v>
@@ -27245,7 +27241,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" s="45">
         <f t="shared" si="384"/>
         <v>45705</v>
@@ -27286,7 +27282,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" s="45">
         <f t="shared" si="384"/>
         <v>45706</v>
@@ -27327,7 +27323,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A205" s="45">
         <f t="shared" si="384"/>
         <v>45707</v>
@@ -27368,7 +27364,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A206" s="45">
         <f t="shared" si="384"/>
         <v>45708</v>
@@ -27409,7 +27405,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A207" s="45">
         <f t="shared" si="384"/>
         <v>45709</v>
@@ -27450,7 +27446,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" s="45">
         <f t="shared" si="384"/>
         <v>45710</v>
@@ -27491,7 +27487,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A209" s="45">
         <f t="shared" si="384"/>
         <v>45711</v>
@@ -27532,7 +27528,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A210" s="45">
         <f t="shared" si="384"/>
         <v>45712</v>
@@ -27573,7 +27569,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A211" s="45">
         <f t="shared" si="384"/>
         <v>45713</v>
@@ -27614,7 +27610,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A212" s="45">
         <f t="shared" si="384"/>
         <v>45714</v>
@@ -27655,7 +27651,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A213" s="45">
         <f t="shared" si="384"/>
         <v>45715</v>
@@ -27696,7 +27692,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A214" s="45">
         <f t="shared" si="384"/>
         <v>45716</v>
@@ -27737,7 +27733,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A215" s="45"/>
       <c r="B215" s="34"/>
       <c r="C215" s="25"/>
@@ -27754,7 +27750,7 @@
       <c r="N215" s="24"/>
       <c r="O215" s="32"/>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A216" s="37"/>
       <c r="B216" s="37"/>
       <c r="C216" s="26"/>
@@ -27769,7 +27765,7 @@
       <c r="M216" s="26"/>
       <c r="N216" s="26"/>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A217" s="48" t="s">
         <v>10</v>
       </c>
@@ -27820,7 +27816,7 @@
       </c>
       <c r="N217" s="27"/>
     </row>
-    <row r="218" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="40" t="s">
         <v>11</v>
       </c>
@@ -27871,7 +27867,7 @@
       </c>
       <c r="N218" s="27"/>
     </row>
-    <row r="219" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="20" t="s">
         <v>12</v>
       </c>
@@ -27922,7 +27918,7 @@
       </c>
       <c r="N219" s="27"/>
     </row>
-    <row r="220" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="20" t="s">
         <v>13</v>
       </c>
@@ -27973,7 +27969,7 @@
       </c>
       <c r="N220" s="27"/>
     </row>
-    <row r="221" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="20" t="s">
         <v>14</v>
       </c>
@@ -28024,7 +28020,7 @@
       </c>
       <c r="N221" s="27"/>
     </row>
-    <row r="222" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="20" t="s">
         <v>15</v>
       </c>
@@ -28075,7 +28071,7 @@
       </c>
       <c r="N222" s="27"/>
     </row>
-    <row r="223" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="20" t="s">
         <v>16</v>
       </c>
@@ -28126,7 +28122,7 @@
       </c>
       <c r="N223" s="27"/>
     </row>
-    <row r="224" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="20" t="s">
         <v>17</v>
       </c>
@@ -28144,7 +28140,7 @@
       <c r="M224" s="27"/>
       <c r="N224" s="27"/>
     </row>
-    <row r="225" spans="1:14" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:14" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="20" t="s">
         <v>18</v>
       </c>
@@ -28195,7 +28191,7 @@
       </c>
       <c r="N225" s="27"/>
     </row>
-    <row r="226" spans="1:14" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:14" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="20" t="s">
         <v>19</v>
       </c>
@@ -28246,7 +28242,7 @@
       </c>
       <c r="N226" s="27"/>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A227" s="20" t="s">
         <v>20</v>
       </c>
@@ -28297,7 +28293,7 @@
       </c>
       <c r="N227" s="27"/>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A228" s="20" t="s">
         <v>21</v>
       </c>
@@ -28348,7 +28344,7 @@
       </c>
       <c r="N228" s="27"/>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A229" s="20" t="s">
         <v>22</v>
       </c>
@@ -28398,7 +28394,7 @@
       </c>
       <c r="N229" s="27"/>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A230" s="20" t="s">
         <v>23</v>
       </c>
@@ -28448,7 +28444,7 @@
       </c>
       <c r="N230" s="27"/>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A231" s="20" t="s">
         <v>24</v>
       </c>
@@ -28498,52 +28494,52 @@
       </c>
       <c r="N231" s="26"/>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A233" s="31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A234" s="31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A235" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A236" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A237" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A238" s="20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A239" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A240" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="22" t="s">
         <v>34</v>
       </c>
@@ -28565,12 +28561,12 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="155" t="s">
         <v>93</v>
       </c>
@@ -28578,7 +28574,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="str">
         <f>'Keswick Flow Alternatives'!C2</f>
         <v>Jul 50%</v>
@@ -28587,7 +28583,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="str">
         <f>'Keswick Flow Alternatives'!D2</f>
         <v>Jul 90%</v>
@@ -28596,7 +28592,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="str">
         <f>'Keswick Flow Alternatives'!E2</f>
         <v>Aug 50%</v>
@@ -28605,7 +28601,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="str">
         <f>'Keswick Flow Alternatives'!F2</f>
         <v>Aug 90%</v>
@@ -28614,7 +28610,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="str">
         <f>'Keswick Flow Alternatives'!G2</f>
         <v>Aug 50% WR1</v>
@@ -28623,7 +28619,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="str">
         <f>'Keswick Flow Alternatives'!H2</f>
         <v>Aug 90% WR1</v>
@@ -28632,7 +28628,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
         <f>'Keswick Flow Alternatives'!I2</f>
         <v>0</v>
@@ -28641,7 +28637,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
         <f>'Keswick Flow Alternatives'!J2</f>
         <v>0</v>
@@ -28650,7 +28646,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
         <f>'Keswick Flow Alternatives'!K2</f>
         <v>0</v>
@@ -28659,7 +28655,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
         <f>'Keswick Flow Alternatives'!L2</f>
         <v>0</v>
@@ -28668,7 +28664,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
         <f>'Keswick Flow Alternatives'!M2</f>
         <v>0</v>
@@ -28677,7 +28673,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
         <f>'Keswick Flow Alternatives'!N2</f>
         <v>0</v>
@@ -28686,22 +28682,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
     </row>
   </sheetData>
@@ -28713,64 +28709,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34AEBA9B-60A1-490D-A063-758B4087F9FB}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52"/>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="54"/>
     </row>
-    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="54"/>
     </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="53"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="53"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="55" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -28785,125 +28781,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA370860-48CD-4B92-B790-82066B2C7AEE}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="8.5546875" style="3"/>
+    <col min="1" max="1" width="13.42578125" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="8.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="36.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="64" t="s">
         <v>97</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
         <v>98</v>
       </c>
       <c r="B11" s="8"/>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="64" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="64" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="64" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="64"/>
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
     </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
     </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="42"/>
     </row>
   </sheetData>
@@ -28917,49 +28913,49 @@
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A1" s="166" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="165" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="166" t="s">
+      <c r="B1" s="165" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="166" t="s">
+      <c r="C1" s="165" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="166" t="s">
+      <c r="D1" s="165" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="166" t="s">
+      <c r="E1" s="165" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="166" t="s">
+      <c r="F1" s="165" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="166" t="s">
+      <c r="G1" s="165" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="166" t="s">
+      <c r="H1" s="165" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="166" t="s">
+      <c r="I1" s="165" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="166" t="s">
+      <c r="J1" s="165" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="169" t="s">
+      <c r="K1" s="168" t="s">
         <v>63</v>
       </c>
       <c r="L1" s="67"/>
       <c r="M1" s="67"/>
-      <c r="N1" s="172" t="s">
+      <c r="N1" s="156" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="173"/>
-      <c r="P1" s="176" t="s">
+      <c r="O1" s="157"/>
+      <c r="P1" s="160" t="s">
         <v>65</v>
       </c>
       <c r="Q1" s="68">
@@ -29001,23 +28997,23 @@
       <c r="AI1" s="67"/>
       <c r="AJ1" s="67"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A2" s="167"/>
-      <c r="B2" s="167"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167"/>
-      <c r="I2" s="167"/>
-      <c r="J2" s="167"/>
-      <c r="K2" s="170"/>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="166"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="166"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="169"/>
       <c r="L2" s="67"/>
       <c r="M2" s="67"/>
-      <c r="N2" s="174"/>
-      <c r="O2" s="175"/>
-      <c r="P2" s="177"/>
+      <c r="N2" s="158"/>
+      <c r="O2" s="159"/>
+      <c r="P2" s="161"/>
       <c r="Q2" s="75">
         <v>45445</v>
       </c>
@@ -29057,36 +29053,36 @@
       <c r="AI2" s="67"/>
       <c r="AJ2" s="67"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A3" s="167"/>
-      <c r="B3" s="167"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-      <c r="I3" s="167"/>
-      <c r="J3" s="167"/>
-      <c r="K3" s="170"/>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="166"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="169"/>
       <c r="L3" s="67"/>
       <c r="M3" s="67"/>
-      <c r="N3" s="178" t="s">
-        <v>66</v>
-      </c>
-      <c r="O3" s="179"/>
-      <c r="P3" s="180"/>
-      <c r="Q3" s="160" t="s">
+      <c r="N3" s="162" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="163"/>
+      <c r="P3" s="164"/>
+      <c r="Q3" s="171" t="s">
         <v>67</v>
       </c>
-      <c r="R3" s="160"/>
-      <c r="S3" s="160"/>
-      <c r="T3" s="160"/>
-      <c r="U3" s="160"/>
-      <c r="V3" s="160"/>
-      <c r="W3" s="160"/>
-      <c r="X3" s="160"/>
-      <c r="Y3" s="161"/>
+      <c r="R3" s="171"/>
+      <c r="S3" s="171"/>
+      <c r="T3" s="171"/>
+      <c r="U3" s="171"/>
+      <c r="V3" s="171"/>
+      <c r="W3" s="171"/>
+      <c r="X3" s="171"/>
+      <c r="Y3" s="172"/>
       <c r="Z3" s="80"/>
       <c r="AA3" s="80"/>
       <c r="AB3" s="80"/>
@@ -29099,18 +29095,18 @@
       <c r="AI3" s="80"/>
       <c r="AJ3" s="80"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A4" s="168"/>
-      <c r="B4" s="168"/>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="168"/>
-      <c r="G4" s="168"/>
-      <c r="H4" s="168"/>
-      <c r="I4" s="168"/>
-      <c r="J4" s="168"/>
-      <c r="K4" s="171"/>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="167"/>
+      <c r="B4" s="167"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="167"/>
+      <c r="I4" s="167"/>
+      <c r="J4" s="167"/>
+      <c r="K4" s="170"/>
       <c r="L4" s="67"/>
       <c r="M4" s="81" t="s">
         <v>66</v>
@@ -29118,10 +29114,10 @@
       <c r="N4" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="O4" s="162" t="s">
+      <c r="O4" s="173" t="s">
         <v>69</v>
       </c>
-      <c r="P4" s="163"/>
+      <c r="P4" s="174"/>
       <c r="Q4" s="83">
         <v>8700</v>
       </c>
@@ -29161,7 +29157,7 @@
       <c r="AI4" s="67"/>
       <c r="AJ4" s="67"/>
     </row>
-    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="88">
         <v>1</v>
       </c>
@@ -29204,10 +29200,10 @@
       <c r="N5" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="O5" s="164">
+      <c r="O5" s="175">
         <v>26</v>
       </c>
-      <c r="P5" s="165"/>
+      <c r="P5" s="176"/>
       <c r="Q5" s="70">
         <v>26</v>
       </c>
@@ -29247,7 +29243,7 @@
       <c r="AI5" s="67"/>
       <c r="AJ5" s="67"/>
     </row>
-    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="88">
         <v>2</v>
       </c>
@@ -29290,10 +29286,10 @@
       <c r="N6" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="O6" s="156">
+      <c r="O6" s="177">
         <v>27</v>
       </c>
-      <c r="P6" s="157"/>
+      <c r="P6" s="178"/>
       <c r="Q6" s="100" t="s">
         <v>66</v>
       </c>
@@ -29333,7 +29329,7 @@
       <c r="AI6" s="67"/>
       <c r="AJ6" s="67"/>
     </row>
-    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="88">
         <v>3</v>
       </c>
@@ -29376,10 +29372,10 @@
       <c r="N7" s="110" t="s">
         <v>75</v>
       </c>
-      <c r="O7" s="156">
+      <c r="O7" s="177">
         <v>23</v>
       </c>
-      <c r="P7" s="157"/>
+      <c r="P7" s="178"/>
       <c r="Q7" s="100" t="s">
         <v>66</v>
       </c>
@@ -29421,7 +29417,7 @@
       <c r="AI7" s="67"/>
       <c r="AJ7" s="67"/>
     </row>
-    <row r="8" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="88">
         <v>4</v>
       </c>
@@ -29464,10 +29460,10 @@
       <c r="N8" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="O8" s="156">
+      <c r="O8" s="177">
         <v>13</v>
       </c>
-      <c r="P8" s="157"/>
+      <c r="P8" s="178"/>
       <c r="Q8" s="100" t="s">
         <v>66</v>
       </c>
@@ -29509,7 +29505,7 @@
       <c r="AI8" s="67"/>
       <c r="AJ8" s="67"/>
     </row>
-    <row r="9" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="88">
         <v>5</v>
       </c>
@@ -29552,10 +29548,10 @@
       <c r="N9" s="110" t="s">
         <v>79</v>
       </c>
-      <c r="O9" s="156">
+      <c r="O9" s="177">
         <v>22</v>
       </c>
-      <c r="P9" s="157"/>
+      <c r="P9" s="178"/>
       <c r="Q9" s="100" t="s">
         <v>66</v>
       </c>
@@ -29595,7 +29591,7 @@
       <c r="AI9" s="67"/>
       <c r="AJ9" s="67"/>
     </row>
-    <row r="10" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="88">
         <v>6</v>
       </c>
@@ -29638,10 +29634,10 @@
       <c r="N10" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="O10" s="156">
+      <c r="O10" s="177">
         <v>10</v>
       </c>
-      <c r="P10" s="157"/>
+      <c r="P10" s="178"/>
       <c r="Q10" s="100" t="s">
         <v>66</v>
       </c>
@@ -29681,7 +29677,7 @@
       <c r="AI10" s="67"/>
       <c r="AJ10" s="67"/>
     </row>
-    <row r="11" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="88">
         <v>7</v>
       </c>
@@ -29724,10 +29720,10 @@
       <c r="N11" s="110" t="s">
         <v>82</v>
       </c>
-      <c r="O11" s="156">
+      <c r="O11" s="177">
         <v>23</v>
       </c>
-      <c r="P11" s="157"/>
+      <c r="P11" s="178"/>
       <c r="Q11" s="100" t="s">
         <v>66</v>
       </c>
@@ -29767,7 +29763,7 @@
       <c r="AI11" s="67"/>
       <c r="AJ11" s="67"/>
     </row>
-    <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="88">
         <v>8</v>
       </c>
@@ -29810,10 +29806,10 @@
       <c r="N12" s="110" t="s">
         <v>83</v>
       </c>
-      <c r="O12" s="156">
+      <c r="O12" s="177">
         <v>34</v>
       </c>
-      <c r="P12" s="157"/>
+      <c r="P12" s="178"/>
       <c r="Q12" s="100" t="s">
         <v>66</v>
       </c>
@@ -29853,7 +29849,7 @@
       <c r="AI12" s="67"/>
       <c r="AJ12" s="67"/>
     </row>
-    <row r="13" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="88">
         <v>9</v>
       </c>
@@ -29896,10 +29892,10 @@
       <c r="N13" s="110" t="s">
         <v>84</v>
       </c>
-      <c r="O13" s="156">
+      <c r="O13" s="177">
         <v>26</v>
       </c>
-      <c r="P13" s="157"/>
+      <c r="P13" s="178"/>
       <c r="Q13" s="100" t="s">
         <v>66</v>
       </c>
@@ -29939,7 +29935,7 @@
       <c r="AI13" s="67"/>
       <c r="AJ13" s="67"/>
     </row>
-    <row r="14" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="88">
         <v>10</v>
       </c>
@@ -29982,10 +29978,10 @@
       <c r="N14" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="O14" s="156">
+      <c r="O14" s="177">
         <v>25</v>
       </c>
-      <c r="P14" s="157"/>
+      <c r="P14" s="178"/>
       <c r="Q14" s="100" t="s">
         <v>66</v>
       </c>
@@ -30027,7 +30023,7 @@
       <c r="AI14" s="67"/>
       <c r="AJ14" s="67"/>
     </row>
-    <row r="15" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="88">
         <v>11</v>
       </c>
@@ -30070,10 +30066,10 @@
       <c r="N15" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="O15" s="156">
+      <c r="O15" s="177">
         <v>27</v>
       </c>
-      <c r="P15" s="157"/>
+      <c r="P15" s="178"/>
       <c r="Q15" s="100" t="s">
         <v>66</v>
       </c>
@@ -30115,7 +30111,7 @@
       <c r="AI15" s="67"/>
       <c r="AJ15" s="67"/>
     </row>
-    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="88">
         <v>12</v>
       </c>
@@ -30158,10 +30154,10 @@
       <c r="N16" s="110" t="s">
         <v>87</v>
       </c>
-      <c r="O16" s="156">
+      <c r="O16" s="177">
         <v>18</v>
       </c>
-      <c r="P16" s="157"/>
+      <c r="P16" s="178"/>
       <c r="Q16" s="100" t="s">
         <v>66</v>
       </c>
@@ -30201,7 +30197,7 @@
       <c r="AI16" s="67"/>
       <c r="AJ16" s="67"/>
     </row>
-    <row r="17" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="88">
         <v>13</v>
       </c>
@@ -30244,10 +30240,10 @@
       <c r="N17" s="110" t="s">
         <v>88</v>
       </c>
-      <c r="O17" s="156">
+      <c r="O17" s="177">
         <v>34</v>
       </c>
-      <c r="P17" s="157"/>
+      <c r="P17" s="178"/>
       <c r="Q17" s="100" t="s">
         <v>66</v>
       </c>
@@ -30287,7 +30283,7 @@
       <c r="AI17" s="67"/>
       <c r="AJ17" s="67"/>
     </row>
-    <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="88">
         <v>14</v>
       </c>
@@ -30330,10 +30326,10 @@
       <c r="N18" s="110" t="s">
         <v>90</v>
       </c>
-      <c r="O18" s="156">
+      <c r="O18" s="177">
         <v>14</v>
       </c>
-      <c r="P18" s="157"/>
+      <c r="P18" s="178"/>
       <c r="Q18" s="100" t="s">
         <v>66</v>
       </c>
@@ -30375,7 +30371,7 @@
       <c r="AI18" s="67"/>
       <c r="AJ18" s="67"/>
     </row>
-    <row r="19" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="88">
         <v>15</v>
       </c>
@@ -30418,10 +30414,10 @@
       <c r="N19" s="110" t="s">
         <v>91</v>
       </c>
-      <c r="O19" s="156">
+      <c r="O19" s="177">
         <v>16</v>
       </c>
-      <c r="P19" s="157"/>
+      <c r="P19" s="178"/>
       <c r="Q19" s="100" t="s">
         <v>66</v>
       </c>
@@ -30463,7 +30459,7 @@
       <c r="AI19" s="67"/>
       <c r="AJ19" s="67"/>
     </row>
-    <row r="20" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="88">
         <v>16</v>
       </c>
@@ -30506,10 +30502,10 @@
       <c r="N20" s="110" t="s">
         <v>92</v>
       </c>
-      <c r="O20" s="156">
+      <c r="O20" s="177">
         <v>24</v>
       </c>
-      <c r="P20" s="157"/>
+      <c r="P20" s="178"/>
       <c r="Q20" s="100" t="s">
         <v>66</v>
       </c>
@@ -30549,7 +30545,7 @@
       <c r="AI20" s="67"/>
       <c r="AJ20" s="67"/>
     </row>
-    <row r="21" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="88" t="s">
         <v>66</v>
       </c>
@@ -30592,10 +30588,10 @@
       <c r="N21" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="O21" s="156" t="s">
-        <v>66</v>
-      </c>
-      <c r="P21" s="157"/>
+      <c r="O21" s="177" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" s="178"/>
       <c r="Q21" s="100" t="s">
         <v>66</v>
       </c>
@@ -30635,7 +30631,7 @@
       <c r="AI21" s="67"/>
       <c r="AJ21" s="67"/>
     </row>
-    <row r="22" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="88" t="s">
         <v>66</v>
       </c>
@@ -30678,10 +30674,10 @@
       <c r="N22" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="O22" s="156" t="s">
-        <v>66</v>
-      </c>
-      <c r="P22" s="157"/>
+      <c r="O22" s="177" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22" s="178"/>
       <c r="Q22" s="100" t="s">
         <v>66</v>
       </c>
@@ -30721,7 +30717,7 @@
       <c r="AI22" s="67"/>
       <c r="AJ22" s="67"/>
     </row>
-    <row r="23" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="88" t="s">
         <v>66</v>
       </c>
@@ -30764,10 +30760,10 @@
       <c r="N23" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="O23" s="156" t="s">
-        <v>66</v>
-      </c>
-      <c r="P23" s="157"/>
+      <c r="O23" s="177" t="s">
+        <v>66</v>
+      </c>
+      <c r="P23" s="178"/>
       <c r="Q23" s="100" t="s">
         <v>66</v>
       </c>
@@ -30807,7 +30803,7 @@
       <c r="AI23" s="67"/>
       <c r="AJ23" s="67"/>
     </row>
-    <row r="24" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="88" t="s">
         <v>66</v>
       </c>
@@ -30850,10 +30846,10 @@
       <c r="N24" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="O24" s="156" t="s">
-        <v>66</v>
-      </c>
-      <c r="P24" s="157"/>
+      <c r="O24" s="177" t="s">
+        <v>66</v>
+      </c>
+      <c r="P24" s="178"/>
       <c r="Q24" s="100" t="s">
         <v>66</v>
       </c>
@@ -30893,7 +30889,7 @@
       <c r="AI24" s="67"/>
       <c r="AJ24" s="67"/>
     </row>
-    <row r="25" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="88" t="s">
         <v>66</v>
       </c>
@@ -30936,10 +30932,10 @@
       <c r="N25" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="O25" s="156" t="s">
-        <v>66</v>
-      </c>
-      <c r="P25" s="157"/>
+      <c r="O25" s="177" t="s">
+        <v>66</v>
+      </c>
+      <c r="P25" s="178"/>
       <c r="Q25" s="100" t="s">
         <v>66</v>
       </c>
@@ -30979,7 +30975,7 @@
       <c r="AI25" s="67"/>
       <c r="AJ25" s="67"/>
     </row>
-    <row r="26" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="88" t="s">
         <v>66</v>
       </c>
@@ -31022,10 +31018,10 @@
       <c r="N26" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="O26" s="158" t="s">
-        <v>66</v>
-      </c>
-      <c r="P26" s="159"/>
+      <c r="O26" s="179" t="s">
+        <v>66</v>
+      </c>
+      <c r="P26" s="180"/>
       <c r="Q26" s="127" t="s">
         <v>66</v>
       </c>
@@ -31065,7 +31061,7 @@
       <c r="AI26" s="67"/>
       <c r="AJ26" s="67"/>
     </row>
-    <row r="27" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="131" t="s">
         <v>66</v>
       </c>
@@ -31153,7 +31149,7 @@
       <c r="AI27" s="67"/>
       <c r="AJ27" s="67"/>
     </row>
-    <row r="28" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="131" t="s">
         <v>66</v>
       </c>
@@ -31241,7 +31237,7 @@
       <c r="AI28" s="67"/>
       <c r="AJ28" s="67"/>
     </row>
-    <row r="29" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="131" t="s">
         <v>66</v>
       </c>
@@ -31329,7 +31325,7 @@
       <c r="AI29" s="67"/>
       <c r="AJ29" s="67"/>
     </row>
-    <row r="30" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="131" t="s">
         <v>66</v>
       </c>
@@ -31417,7 +31413,7 @@
       <c r="AI30" s="67"/>
       <c r="AJ30" s="67"/>
     </row>
-    <row r="31" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="131" t="s">
         <v>66</v>
       </c>
@@ -31505,7 +31501,7 @@
       <c r="AI31" s="67"/>
       <c r="AJ31" s="67"/>
     </row>
-    <row r="32" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="143" t="s">
         <v>66</v>
       </c>
@@ -31593,7 +31589,7 @@
       <c r="AI32" s="67"/>
       <c r="AJ32" s="67"/>
     </row>
-    <row r="33" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="143" t="s">
         <v>66</v>
       </c>
@@ -31681,7 +31677,7 @@
       <c r="AI33" s="67"/>
       <c r="AJ33" s="67"/>
     </row>
-    <row r="34" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="143" t="s">
         <v>66</v>
       </c>
@@ -31769,7 +31765,7 @@
       <c r="AI34" s="67"/>
       <c r="AJ34" s="67"/>
     </row>
-    <row r="35" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="143" t="s">
         <v>66</v>
       </c>
@@ -31857,7 +31853,7 @@
       <c r="AI35" s="67"/>
       <c r="AJ35" s="67"/>
     </row>
-    <row r="36" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="143" t="s">
         <v>66</v>
       </c>
@@ -31945,7 +31941,7 @@
       <c r="AI36" s="67"/>
       <c r="AJ36" s="67"/>
     </row>
-    <row r="37" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="148" t="s">
         <v>66</v>
       </c>
@@ -32033,7 +32029,7 @@
       <c r="AI37" s="67"/>
       <c r="AJ37" s="67"/>
     </row>
-    <row r="38" spans="1:36" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="148" t="s">
         <v>66</v>
       </c>
@@ -32121,7 +32117,7 @@
       <c r="AI38" s="67"/>
       <c r="AJ38" s="67"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="148" t="s">
         <v>66</v>
       </c>
@@ -32209,7 +32205,7 @@
       <c r="AI39" s="67"/>
       <c r="AJ39" s="67"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="148" t="s">
         <v>66</v>
       </c>
@@ -32297,7 +32293,7 @@
       <c r="AI40" s="67"/>
       <c r="AJ40" s="67"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="148" t="s">
         <v>66</v>
       </c>
@@ -32385,7 +32381,7 @@
       <c r="AI41" s="67"/>
       <c r="AJ41" s="67"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="148" t="s">
         <v>66</v>
       </c>
@@ -32473,7 +32469,7 @@
       <c r="AI42" s="67"/>
       <c r="AJ42" s="67"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="148" t="s">
         <v>66</v>
       </c>
@@ -32561,7 +32557,7 @@
       <c r="AI43" s="67"/>
       <c r="AJ43" s="67"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="148" t="s">
         <v>66</v>
       </c>
@@ -32649,7 +32645,7 @@
       <c r="AI44" s="67"/>
       <c r="AJ44" s="67"/>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="148" t="s">
         <v>66</v>
       </c>
@@ -32737,7 +32733,7 @@
       <c r="AI45" s="67"/>
       <c r="AJ45" s="67"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="148" t="s">
         <v>66</v>
       </c>
@@ -32825,7 +32821,7 @@
       <c r="AI46" s="67"/>
       <c r="AJ46" s="67"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="148" t="s">
         <v>66</v>
       </c>
@@ -32913,7 +32909,7 @@
       <c r="AI47" s="67"/>
       <c r="AJ47" s="67"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="148" t="s">
         <v>66</v>
       </c>
@@ -33001,7 +32997,7 @@
       <c r="AI48" s="67"/>
       <c r="AJ48" s="67"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="148" t="s">
         <v>66</v>
       </c>
@@ -33089,7 +33085,7 @@
       <c r="AI49" s="67"/>
       <c r="AJ49" s="67"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="148" t="s">
         <v>66</v>
       </c>
@@ -33177,7 +33173,7 @@
       <c r="AI50" s="67"/>
       <c r="AJ50" s="67"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="148" t="s">
         <v>66</v>
       </c>
@@ -33265,7 +33261,7 @@
       <c r="AI51" s="67"/>
       <c r="AJ51" s="67"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="148" t="s">
         <v>66</v>
       </c>
@@ -33353,7 +33349,7 @@
       <c r="AI52" s="67"/>
       <c r="AJ52" s="67"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="148" t="s">
         <v>66</v>
       </c>
@@ -33441,7 +33437,7 @@
       <c r="AI53" s="67"/>
       <c r="AJ53" s="67"/>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="148" t="s">
         <v>66</v>
       </c>
@@ -33529,7 +33525,7 @@
       <c r="AI54" s="67"/>
       <c r="AJ54" s="67"/>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="148" t="s">
         <v>66</v>
       </c>
@@ -33617,7 +33613,7 @@
       <c r="AI55" s="67"/>
       <c r="AJ55" s="67"/>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="148" t="s">
         <v>66</v>
       </c>
@@ -33705,7 +33701,7 @@
       <c r="AI56" s="67"/>
       <c r="AJ56" s="67"/>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="148" t="s">
         <v>66</v>
       </c>
@@ -33793,7 +33789,7 @@
       <c r="AI57" s="67"/>
       <c r="AJ57" s="67"/>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="148" t="s">
         <v>66</v>
       </c>
@@ -33881,7 +33877,7 @@
       <c r="AI58" s="67"/>
       <c r="AJ58" s="67"/>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="148" t="s">
         <v>66</v>
       </c>
@@ -33969,7 +33965,7 @@
       <c r="AI59" s="67"/>
       <c r="AJ59" s="67"/>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="148" t="s">
         <v>66</v>
       </c>
@@ -34057,7 +34053,7 @@
       <c r="AI60" s="67"/>
       <c r="AJ60" s="67"/>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="148" t="s">
         <v>66</v>
       </c>
@@ -34145,7 +34141,7 @@
       <c r="AI61" s="67"/>
       <c r="AJ61" s="67"/>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="148" t="s">
         <v>66</v>
       </c>
@@ -34233,7 +34229,7 @@
       <c r="AI62" s="67"/>
       <c r="AJ62" s="67"/>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="148" t="s">
         <v>66</v>
       </c>
@@ -34321,7 +34317,7 @@
       <c r="AI63" s="67"/>
       <c r="AJ63" s="67"/>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="148" t="s">
         <v>66</v>
       </c>
@@ -34409,7 +34405,7 @@
       <c r="AI64" s="67"/>
       <c r="AJ64" s="67"/>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="148" t="s">
         <v>66</v>
       </c>
@@ -34497,7 +34493,7 @@
       <c r="AI65" s="67"/>
       <c r="AJ65" s="67"/>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="148" t="s">
         <v>66</v>
       </c>
@@ -34585,7 +34581,7 @@
       <c r="AI66" s="67"/>
       <c r="AJ66" s="67"/>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="148" t="s">
         <v>66</v>
       </c>
@@ -34673,7 +34669,7 @@
       <c r="AI67" s="67"/>
       <c r="AJ67" s="67"/>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="148" t="s">
         <v>66</v>
       </c>
@@ -34761,7 +34757,7 @@
       <c r="AI68" s="67"/>
       <c r="AJ68" s="67"/>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="148" t="s">
         <v>66</v>
       </c>
@@ -34849,7 +34845,7 @@
       <c r="AI69" s="67"/>
       <c r="AJ69" s="67"/>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="148" t="s">
         <v>66</v>
       </c>
@@ -34937,7 +34933,7 @@
       <c r="AI70" s="67"/>
       <c r="AJ70" s="67"/>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="148" t="s">
         <v>66</v>
       </c>
@@ -35027,20 +35023,14 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="F1:F4"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="G1:G4"/>
-    <mergeCell ref="H1:H4"/>
-    <mergeCell ref="I1:I4"/>
-    <mergeCell ref="J1:J4"/>
-    <mergeCell ref="K1:K4"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
     <mergeCell ref="Q3:Y3"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="O5:P5"/>
@@ -35057,14 +35047,20 @@
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O17:P17"/>
     <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="F1:F4"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="G1:G4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="I1:I4"/>
+    <mergeCell ref="J1:J4"/>
+    <mergeCell ref="K1:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>